<commit_message>
Fix DSL for Extract
</commit_message>
<xml_diff>
--- a/docs/base/DataLists.xlsx
+++ b/docs/base/DataLists.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="178">
   <si>
     <t xml:space="preserve">Nama File</t>
   </si>
@@ -42,6 +42,9 @@
     <t xml:space="preserve">Waktu Kejadian</t>
   </si>
   <si>
+    <t xml:space="preserve">Tempat</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pelaku</t>
   </si>
   <si>
@@ -57,12 +60,6 @@
     <t xml:space="preserve">Pasal</t>
   </si>
   <si>
-    <t xml:space="preserve">Petugas Pencatat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jabatan</t>
-  </si>
-  <si>
     <t xml:space="preserve">Prod1.docx</t>
   </si>
   <si>
@@ -93,12 +90,6 @@
     <t xml:space="preserve">362 KUHP</t>
   </si>
   <si>
-    <t xml:space="preserve">BUDI NUGROHO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIPTU NRP 71110231</t>
-  </si>
-  <si>
     <t xml:space="preserve">Prod2.docx</t>
   </si>
   <si>
@@ -132,12 +123,6 @@
     <t xml:space="preserve">351 KUHP</t>
   </si>
   <si>
-    <t xml:space="preserve">Santoso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIPTU NRP 71110224</t>
-  </si>
-  <si>
     <t xml:space="preserve">Prod3.docx</t>
   </si>
   <si>
@@ -150,6 +135,9 @@
     <t xml:space="preserve">-</t>
   </si>
   <si>
+    <t xml:space="preserve">Belum diketahui</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sutini</t>
   </si>
   <si>
@@ -162,12 +150,6 @@
     <t xml:space="preserve">338 KUHP</t>
   </si>
   <si>
-    <t xml:space="preserve">Rahmat Hidayat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIPTU NRP 61110332</t>
-  </si>
-  <si>
     <t xml:space="preserve">Prod4.docx</t>
   </si>
   <si>
@@ -196,12 +178,6 @@
   </si>
   <si>
     <t xml:space="preserve">285 KUHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sukirman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIPTU NRP 51210443</t>
   </si>
   <si>
     <t xml:space="preserve">Prod5.docx</t>
@@ -692,28 +668,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.0485829959514"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="34.2145748987854"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="19.4372469635628"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.9311740890688"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="17.3400809716599"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="14.6963562753036"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="19.2186234817814"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="28.3643724696356"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="19.8461538461538"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="16.4615384615385"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="20.0971659919028"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="59.1295546558704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="2" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="59.663967611336"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -753,889 +729,754 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="I5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="J7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="J10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="J12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="I13" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>37</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="H15" s="2" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>56</v>
+        <v>133</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>41</v>
+        <v>138</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>147</v>
+        <v>37</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J16" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>151</v>
+        <v>90</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="J17" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>34</v>
+        <v>150</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>92</v>
+        <v>152</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="J20" s="2" t="s">
+      <c r="K20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>171</v>
+        <v>37</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="J21" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="2" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>175</v>
+        <v>37</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="J22" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="L23" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>